<commit_message>
updated DropletSeparation.py and GridSegmentation.py for matplotlib update and rerun example. Added screenshots for doc.
</commit_message>
<xml_diff>
--- a/output/HG2A_30s/DropletsIntensity.xlsx
+++ b/output/HG2A_30s/DropletsIntensity.xlsx
@@ -415,40 +415,40 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>225.5774647887324</v>
+        <v>210.3866666666667</v>
       </c>
       <c r="C2">
-        <v>214.7323943661972</v>
+        <v>201.8933333333333</v>
       </c>
       <c r="D2">
-        <v>305.3802816901408</v>
+        <v>282.92</v>
       </c>
       <c r="E2">
-        <v>253.7887323943662</v>
+        <v>240.1733333333333</v>
       </c>
       <c r="F2">
-        <v>268.056338028169</v>
+        <v>252.5333333333333</v>
       </c>
       <c r="G2">
-        <v>275.3098591549296</v>
+        <v>257.3199999999999</v>
       </c>
       <c r="H2">
-        <v>516.9859154929577</v>
+        <v>488.4533333333334</v>
       </c>
       <c r="I2">
-        <v>496.5633802816901</v>
+        <v>466.96</v>
       </c>
       <c r="J2">
-        <v>511.6338028169014</v>
+        <v>482.64</v>
       </c>
       <c r="K2">
-        <v>449.0845070422535</v>
+        <v>423.7066666666666</v>
       </c>
       <c r="L2">
-        <v>410.225352112676</v>
+        <v>385.4133333333333</v>
       </c>
       <c r="M2">
-        <v>408.6760563380282</v>
+        <v>382.3333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -456,40 +456,40 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>159.7746478873239</v>
+        <v>150.1066666666667</v>
       </c>
       <c r="C3">
-        <v>225.6901408450704</v>
+        <v>210.3066666666666</v>
       </c>
       <c r="D3">
-        <v>277.4507042253521</v>
+        <v>259.7333333333333</v>
       </c>
       <c r="E3">
-        <v>276.9436619718309</v>
+        <v>261.9066666666666</v>
       </c>
       <c r="F3">
-        <v>273.2676056338028</v>
+        <v>257.4533333333333</v>
       </c>
       <c r="G3">
-        <v>281.7323943661971</v>
+        <v>264.04</v>
       </c>
       <c r="H3">
-        <v>521.8450704225352</v>
+        <v>493.2666666666667</v>
       </c>
       <c r="I3">
-        <v>494.6197183098592</v>
+        <v>468.6</v>
       </c>
       <c r="J3">
-        <v>539.1267605633802</v>
+        <v>510.3200000000001</v>
       </c>
       <c r="K3">
-        <v>465.8450704225352</v>
+        <v>439.5333333333333</v>
       </c>
       <c r="L3">
-        <v>461.2535211267606</v>
+        <v>435.1466666666666</v>
       </c>
       <c r="M3">
-        <v>391.4225352112676</v>
+        <v>368.5466666666667</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -497,40 +497,40 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>105.1408450704225</v>
+        <v>99.13333333333333</v>
       </c>
       <c r="C4">
-        <v>124.1690140845071</v>
+        <v>118.4</v>
       </c>
       <c r="D4">
-        <v>134.6056338028169</v>
+        <v>128.0533333333333</v>
       </c>
       <c r="E4">
-        <v>142.830985915493</v>
+        <v>134.12</v>
       </c>
       <c r="F4">
-        <v>145.0281690140845</v>
+        <v>137.9333333333333</v>
       </c>
       <c r="G4">
-        <v>154.4225352112676</v>
+        <v>144.2533333333333</v>
       </c>
       <c r="H4">
-        <v>339.6901408450704</v>
+        <v>318.5066666666667</v>
       </c>
       <c r="I4">
-        <v>321.056338028169</v>
+        <v>304.16</v>
       </c>
       <c r="J4">
-        <v>306.0281690140845</v>
+        <v>289.24</v>
       </c>
       <c r="K4">
-        <v>291.6338028169014</v>
+        <v>279.04</v>
       </c>
       <c r="L4">
-        <v>287.4647887323944</v>
+        <v>270.2666666666667</v>
       </c>
       <c r="M4">
-        <v>246.3380281690141</v>
+        <v>229.68</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -538,40 +538,40 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>51.19718309859155</v>
+        <v>47.66666666666666</v>
       </c>
       <c r="C5">
-        <v>61.16901408450705</v>
+        <v>53.65333333333334</v>
       </c>
       <c r="D5">
-        <v>81.57746478873239</v>
+        <v>76.21333333333332</v>
       </c>
       <c r="E5">
-        <v>59.28169014084507</v>
+        <v>57.12</v>
       </c>
       <c r="F5">
-        <v>86.47887323943661</v>
+        <v>81.78666666666666</v>
       </c>
       <c r="G5">
-        <v>74.2676056338028</v>
+        <v>69.53333333333333</v>
       </c>
       <c r="H5">
-        <v>273.1549295774648</v>
+        <v>257.1733333333333</v>
       </c>
       <c r="I5">
-        <v>249.0704225352113</v>
+        <v>232.28</v>
       </c>
       <c r="J5">
-        <v>272.4788732394366</v>
+        <v>255.48</v>
       </c>
       <c r="K5">
-        <v>225.3521126760563</v>
+        <v>214.0133333333333</v>
       </c>
       <c r="L5">
-        <v>205.6760563380282</v>
+        <v>194.32</v>
       </c>
       <c r="M5">
-        <v>181.4788732394366</v>
+        <v>168.0133333333333</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -579,40 +579,40 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>44.70422535211267</v>
+        <v>42.25333333333333</v>
       </c>
       <c r="C6">
-        <v>46.87323943661972</v>
+        <v>44.78666666666666</v>
       </c>
       <c r="D6">
-        <v>52.08450704225353</v>
+        <v>49.22666666666667</v>
       </c>
       <c r="E6">
-        <v>51.14084507042254</v>
+        <v>48.53333333333332</v>
       </c>
       <c r="F6">
-        <v>52.26760563380282</v>
+        <v>49.92</v>
       </c>
       <c r="G6">
-        <v>42.63380281690141</v>
+        <v>39.33333333333333</v>
       </c>
       <c r="H6">
-        <v>208.6478873239437</v>
+        <v>194.76</v>
       </c>
       <c r="I6">
-        <v>195.3802816901409</v>
+        <v>183.36</v>
       </c>
       <c r="J6">
-        <v>187.7042253521127</v>
+        <v>175.8</v>
       </c>
       <c r="K6">
-        <v>163.3943661971831</v>
+        <v>153.2933333333333</v>
       </c>
       <c r="L6">
-        <v>147.6901408450704</v>
+        <v>139.8133333333333</v>
       </c>
       <c r="M6">
-        <v>116.056338028169</v>
+        <v>108.5866666666667</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -638,16 +638,16 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>67.33802816901408</v>
+        <v>62.65333333333334</v>
       </c>
       <c r="I7">
-        <v>63.63380281690141</v>
+        <v>58.38666666666666</v>
       </c>
       <c r="J7">
-        <v>64.25352112676056</v>
+        <v>58.56</v>
       </c>
       <c r="K7">
-        <v>39.56338028169013</v>
+        <v>37.12</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -661,40 +661,40 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>254.4507042253521</v>
+        <v>242.2266666666667</v>
       </c>
       <c r="C8">
-        <v>287.4084507042253</v>
+        <v>271.3066666666666</v>
       </c>
       <c r="D8">
-        <v>269.0704225352113</v>
+        <v>254.0133333333333</v>
       </c>
       <c r="E8">
-        <v>239.7605633802817</v>
+        <v>225.68</v>
       </c>
       <c r="F8">
-        <v>233.8309859154929</v>
+        <v>219.4533333333333</v>
       </c>
       <c r="G8">
-        <v>249.1408450704225</v>
+        <v>234.96</v>
       </c>
       <c r="H8">
-        <v>425.3380281690141</v>
+        <v>400.0933333333334</v>
       </c>
       <c r="I8">
-        <v>383.3239436619718</v>
+        <v>361.5466666666667</v>
       </c>
       <c r="J8">
-        <v>386.1408450704225</v>
+        <v>364.0933333333333</v>
       </c>
       <c r="K8">
-        <v>362.0985915492957</v>
+        <v>340.6666666666666</v>
       </c>
       <c r="L8">
-        <v>353.5070422535211</v>
+        <v>331.8933333333333</v>
       </c>
       <c r="M8">
-        <v>364.0704225352113</v>
+        <v>342.88</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -702,40 +702,40 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>136.0422535211268</v>
+        <v>127.24</v>
       </c>
       <c r="C9">
-        <v>255.4225352112676</v>
+        <v>240.88</v>
       </c>
       <c r="D9">
-        <v>231.9859154929577</v>
+        <v>218.64</v>
       </c>
       <c r="E9">
-        <v>203.3239436619718</v>
+        <v>192.76</v>
       </c>
       <c r="F9">
-        <v>197.8450704225352</v>
+        <v>187.3066666666667</v>
       </c>
       <c r="G9">
-        <v>196.6619718309859</v>
+        <v>183.68</v>
       </c>
       <c r="H9">
-        <v>385.3380281690141</v>
+        <v>364.1866666666667</v>
       </c>
       <c r="I9">
-        <v>379.8732394366197</v>
+        <v>357.48</v>
       </c>
       <c r="J9">
-        <v>374.4647887323944</v>
+        <v>352.1333333333333</v>
       </c>
       <c r="K9">
-        <v>351.8028169014084</v>
+        <v>330.5599999999999</v>
       </c>
       <c r="L9">
-        <v>364.4647887323944</v>
+        <v>341.5466666666666</v>
       </c>
       <c r="M9">
-        <v>366.3098591549295</v>
+        <v>344.4533333333333</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -743,40 +743,40 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>26.7887323943662</v>
+        <v>25.25333333333334</v>
       </c>
       <c r="C10">
-        <v>180.2957746478873</v>
+        <v>170.3466666666666</v>
       </c>
       <c r="D10">
-        <v>149.5633802816901</v>
+        <v>141.4933333333333</v>
       </c>
       <c r="E10">
-        <v>127.1690140845071</v>
+        <v>119.7466666666667</v>
       </c>
       <c r="F10">
-        <v>135.7605633802817</v>
+        <v>129.0266666666666</v>
       </c>
       <c r="G10">
-        <v>123.7183098591549</v>
+        <v>117.2133333333333</v>
       </c>
       <c r="H10">
-        <v>330.2676056338028</v>
+        <v>311.5333333333333</v>
       </c>
       <c r="I10">
-        <v>291.5070422535211</v>
+        <v>276.3466666666667</v>
       </c>
       <c r="J10">
-        <v>304.8169014084507</v>
+        <v>285.6799999999999</v>
       </c>
       <c r="K10">
-        <v>282.4647887323944</v>
+        <v>268.04</v>
       </c>
       <c r="L10">
-        <v>265.3098591549295</v>
+        <v>251.76</v>
       </c>
       <c r="M10">
-        <v>265.4366197183099</v>
+        <v>249.5333333333333</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -787,37 +787,37 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>47.38028169014084</v>
+        <v>45.48</v>
       </c>
       <c r="D11">
-        <v>98.69014084507042</v>
+        <v>93.37333333333333</v>
       </c>
       <c r="E11">
-        <v>89.11267605633802</v>
+        <v>83.90666666666667</v>
       </c>
       <c r="F11">
-        <v>62.15492957746478</v>
+        <v>59.64</v>
       </c>
       <c r="G11">
-        <v>34.26760563380282</v>
+        <v>32.53333333333333</v>
       </c>
       <c r="H11">
-        <v>283.2816901408451</v>
+        <v>269</v>
       </c>
       <c r="I11">
-        <v>259.887323943662</v>
+        <v>247.24</v>
       </c>
       <c r="J11">
-        <v>253.5915492957746</v>
+        <v>239.2666666666667</v>
       </c>
       <c r="K11">
-        <v>251.8732394366197</v>
+        <v>239.8133333333333</v>
       </c>
       <c r="L11">
-        <v>251.5915492957746</v>
+        <v>237.52</v>
       </c>
       <c r="M11">
-        <v>217.2816901408451</v>
+        <v>205.1066666666667</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -843,22 +843,22 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>257.4366197183099</v>
+        <v>244.16</v>
       </c>
       <c r="I12">
-        <v>223.8732394366197</v>
+        <v>212.9466666666667</v>
       </c>
       <c r="J12">
-        <v>199.7746478873239</v>
+        <v>188.6266666666667</v>
       </c>
       <c r="K12">
-        <v>194.5774647887324</v>
+        <v>183.6533333333333</v>
       </c>
       <c r="L12">
-        <v>195.5633802816901</v>
+        <v>187.4133333333333</v>
       </c>
       <c r="M12">
-        <v>112.3661971830986</v>
+        <v>105.7866666666667</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -884,19 +884,19 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>190.2112676056338</v>
+        <v>178.2133333333333</v>
       </c>
       <c r="I13">
-        <v>152.3802816901409</v>
+        <v>143.9866666666667</v>
       </c>
       <c r="J13">
-        <v>105.112676056338</v>
+        <v>99.75999999999999</v>
       </c>
       <c r="K13">
-        <v>75.59154929577464</v>
+        <v>72.82666666666667</v>
       </c>
       <c r="L13">
-        <v>43.32394366197183</v>
+        <v>40.88</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -910,37 +910,37 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>162.0140845070422</v>
+        <v>154.72</v>
       </c>
       <c r="D14">
-        <v>119.9718309859155</v>
+        <v>114.92</v>
       </c>
       <c r="E14">
-        <v>130.169014084507</v>
+        <v>124.56</v>
       </c>
       <c r="F14">
-        <v>126.8450704225352</v>
+        <v>120.04</v>
       </c>
       <c r="G14">
-        <v>119.4929577464789</v>
+        <v>112.8933333333333</v>
       </c>
       <c r="H14">
-        <v>256.5352112676056</v>
+        <v>241.84</v>
       </c>
       <c r="I14">
-        <v>219.3802816901409</v>
+        <v>209.72</v>
       </c>
       <c r="J14">
-        <v>208.169014084507</v>
+        <v>198.4933333333333</v>
       </c>
       <c r="K14">
-        <v>206.0704225352113</v>
+        <v>193.4533333333333</v>
       </c>
       <c r="L14">
-        <v>229.5070422535211</v>
+        <v>216.7733333333333</v>
       </c>
       <c r="M14">
-        <v>227.5352112676056</v>
+        <v>214.92</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -951,37 +951,37 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>85.59154929577466</v>
+        <v>77.73333333333332</v>
       </c>
       <c r="D15">
-        <v>94.63380281690141</v>
+        <v>88.46666666666667</v>
       </c>
       <c r="E15">
-        <v>82.12676056338029</v>
+        <v>75.31999999999999</v>
       </c>
       <c r="F15">
-        <v>88.63380281690141</v>
+        <v>84.19999999999999</v>
       </c>
       <c r="G15">
-        <v>104.3802816901408</v>
+        <v>96.88</v>
       </c>
       <c r="H15">
-        <v>268.4366197183098</v>
+        <v>253.9333333333333</v>
       </c>
       <c r="I15">
-        <v>238.7042253521127</v>
+        <v>226.2266666666667</v>
       </c>
       <c r="J15">
-        <v>225.5915492957747</v>
+        <v>211.9333333333333</v>
       </c>
       <c r="K15">
-        <v>223.8028169014084</v>
+        <v>211.7333333333333</v>
       </c>
       <c r="L15">
-        <v>192.9295774647887</v>
+        <v>182.5466666666667</v>
       </c>
       <c r="M15">
-        <v>252.5492957746478</v>
+        <v>239.12</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -992,37 +992,37 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>17.3943661971831</v>
+        <v>16.53333333333333</v>
       </c>
       <c r="D16">
-        <v>22.35211267605634</v>
+        <v>21.33333333333333</v>
       </c>
       <c r="E16">
-        <v>21.80281690140845</v>
+        <v>20.97333333333334</v>
       </c>
       <c r="F16">
-        <v>21.25352112676056</v>
+        <v>20.48</v>
       </c>
       <c r="G16">
-        <v>18.90140845070423</v>
+        <v>16.49333333333333</v>
       </c>
       <c r="H16">
-        <v>169.1408450704225</v>
+        <v>159.4666666666666</v>
       </c>
       <c r="I16">
-        <v>150.3521126760563</v>
+        <v>143.6133333333333</v>
       </c>
       <c r="J16">
-        <v>161.5915492957746</v>
+        <v>153.4</v>
       </c>
       <c r="K16">
-        <v>126.6338028169014</v>
+        <v>120.6933333333333</v>
       </c>
       <c r="L16">
-        <v>130.2112676056338</v>
+        <v>124.5066666666667</v>
       </c>
       <c r="M16">
-        <v>127.0845070422535</v>
+        <v>121.2133333333333</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1036,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>14.95774647887324</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1048,22 +1048,22 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>171.169014084507</v>
+        <v>161.8933333333333</v>
       </c>
       <c r="I17">
-        <v>161.3943661971831</v>
+        <v>153.2533333333333</v>
       </c>
       <c r="J17">
-        <v>162.1830985915493</v>
+        <v>151.9466666666667</v>
       </c>
       <c r="K17">
-        <v>134.0845070422535</v>
+        <v>125.5733333333333</v>
       </c>
       <c r="L17">
-        <v>126.1408450704225</v>
+        <v>120.5733333333333</v>
       </c>
       <c r="M17">
-        <v>125.2535211267606</v>
+        <v>118.9733333333333</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1089,22 +1089,22 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>130.0281690140845</v>
+        <v>122.7466666666667</v>
       </c>
       <c r="I18">
-        <v>137.5492957746479</v>
+        <v>129.76</v>
       </c>
       <c r="J18">
-        <v>165.6338028169014</v>
+        <v>155.6933333333333</v>
       </c>
       <c r="K18">
-        <v>115.9295774647887</v>
+        <v>109.4</v>
       </c>
       <c r="L18">
-        <v>104.5070422535211</v>
+        <v>98.31999999999999</v>
       </c>
       <c r="M18">
-        <v>95.16901408450704</v>
+        <v>90.8</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -1130,22 +1130,22 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <v>44.01408450704226</v>
+        <v>41.65333333333334</v>
       </c>
       <c r="I19">
-        <v>36.56338028169014</v>
+        <v>35.25333333333334</v>
       </c>
       <c r="J19">
-        <v>50.1830985915493</v>
+        <v>47.01333333333334</v>
       </c>
       <c r="K19">
-        <v>42.09859154929578</v>
+        <v>40.54666666666667</v>
       </c>
       <c r="L19">
-        <v>43.52112676056338</v>
+        <v>40.94666666666666</v>
       </c>
       <c r="M19">
-        <v>63.08450704225351</v>
+        <v>60.13333333333333</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -1156,37 +1156,37 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>114.3380281690141</v>
+        <v>107.1466666666666</v>
       </c>
       <c r="D20">
-        <v>231.5774647887324</v>
+        <v>220.3066666666666</v>
       </c>
       <c r="E20">
-        <v>168.7183098591549</v>
+        <v>159.5333333333333</v>
       </c>
       <c r="F20">
-        <v>211.0704225352113</v>
+        <v>199.0133333333333</v>
       </c>
       <c r="G20">
-        <v>201.8028169014084</v>
+        <v>191.52</v>
       </c>
       <c r="H20">
-        <v>454.943661971831</v>
+        <v>433.7333333333333</v>
       </c>
       <c r="I20">
-        <v>462.056338028169</v>
+        <v>435.5333333333333</v>
       </c>
       <c r="J20">
-        <v>526.1971830985915</v>
+        <v>497.52</v>
       </c>
       <c r="K20">
-        <v>529.7746478873239</v>
+        <v>501.9466666666666</v>
       </c>
       <c r="L20">
-        <v>525.4929577464789</v>
+        <v>499.8933333333333</v>
       </c>
       <c r="M20">
-        <v>514.7042253521126</v>
+        <v>489.3466666666667</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -1197,37 +1197,37 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>57.98591549295774</v>
+        <v>54.73333333333333</v>
       </c>
       <c r="D21">
-        <v>244.6760563380282</v>
+        <v>231.9066666666666</v>
       </c>
       <c r="E21">
-        <v>259.9718309859155</v>
+        <v>246.48</v>
       </c>
       <c r="F21">
-        <v>302.5633802816901</v>
+        <v>286.96</v>
       </c>
       <c r="G21">
-        <v>374.1830985915493</v>
+        <v>355.0666666666666</v>
       </c>
       <c r="H21">
-        <v>568.5633802816901</v>
+        <v>539.0933333333334</v>
       </c>
       <c r="I21">
-        <v>550.9859154929577</v>
+        <v>519.4</v>
       </c>
       <c r="J21">
-        <v>542.9859154929577</v>
+        <v>514.1866666666666</v>
       </c>
       <c r="K21">
-        <v>553.0704225352113</v>
+        <v>521.3466666666666</v>
       </c>
       <c r="L21">
-        <v>610.4647887323944</v>
+        <v>578.6133333333332</v>
       </c>
       <c r="M21">
-        <v>595.056338028169</v>
+        <v>564.5866666666667</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -1235,40 +1235,40 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>89.30985915492957</v>
+        <v>83.94666666666666</v>
       </c>
       <c r="C22">
-        <v>41.87323943661971</v>
+        <v>39.2</v>
       </c>
       <c r="D22">
-        <v>185.5070422535211</v>
+        <v>174.68</v>
       </c>
       <c r="E22">
-        <v>223.6338028169014</v>
+        <v>212.7466666666667</v>
       </c>
       <c r="F22">
-        <v>270.6056338028169</v>
+        <v>256.6666666666666</v>
       </c>
       <c r="G22">
-        <v>256.3521126760563</v>
+        <v>244.3066666666667</v>
       </c>
       <c r="H22">
-        <v>471.8450704225352</v>
+        <v>447.6933333333333</v>
       </c>
       <c r="I22">
-        <v>333.056338028169</v>
+        <v>315.1333333333333</v>
       </c>
       <c r="J22">
-        <v>370.6901408450705</v>
+        <v>349.9733333333334</v>
       </c>
       <c r="K22">
-        <v>298.169014084507</v>
+        <v>282.7733333333333</v>
       </c>
       <c r="L22">
-        <v>275.112676056338</v>
+        <v>259.36</v>
       </c>
       <c r="M22">
-        <v>466.6056338028169</v>
+        <v>437.3466666666666</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -1279,37 +1279,37 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <v>22.67605633802817</v>
+        <v>21.38666666666666</v>
       </c>
       <c r="D23">
-        <v>11.92957746478873</v>
+        <v>11.2</v>
       </c>
       <c r="E23">
-        <v>45.2394366197183</v>
+        <v>42.79999999999999</v>
       </c>
       <c r="F23">
-        <v>58.40845070422535</v>
+        <v>54.86666666666666</v>
       </c>
       <c r="G23">
-        <v>163.4084507042253</v>
+        <v>154.7466666666667</v>
       </c>
       <c r="H23">
-        <v>476.2394366197183</v>
+        <v>448.96</v>
       </c>
       <c r="I23">
-        <v>290.8028169014084</v>
+        <v>274.9733333333333</v>
       </c>
       <c r="J23">
-        <v>542.3802816901408</v>
+        <v>506.5866666666666</v>
       </c>
       <c r="K23">
-        <v>304.2816901408451</v>
+        <v>289.1066666666667</v>
       </c>
       <c r="L23">
-        <v>356.1267605633802</v>
+        <v>333.76</v>
       </c>
       <c r="M23">
-        <v>638.8450704225352</v>
+        <v>601.7733333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>